<commit_message>
depot api changed with cleaner structure and misc happend
</commit_message>
<xml_diff>
--- a/sample_budget.xlsx
+++ b/sample_budget.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="54">
   <si>
     <t xml:space="preserve">BudgetID</t>
   </si>
@@ -136,6 +136,9 @@
     <t xml:space="preserve">Diary</t>
   </si>
   <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
     <t xml:space="preserve">DepoBB01F001</t>
   </si>
   <si>
@@ -151,19 +154,31 @@
     <t xml:space="preserve">DU</t>
   </si>
   <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepoBB01F002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepoBB01F003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepoBB01F004</t>
+  </si>
+  <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">DepoBB01F002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepoBB01F003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepoBB01F004</t>
-  </si>
-  <si>
     <t xml:space="preserve">DepoBB01F005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
   </si>
   <si>
     <t xml:space="preserve">DepoBB01F006</t>
@@ -270,10 +285,10 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -625,10 +640,10 @@
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>20</v>
@@ -637,13 +652,13 @@
         <v>10</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>24</v>
@@ -652,7 +667,7 @@
         <v>2023</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,10 +687,10 @@
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>27</v>
@@ -684,13 +699,13 @@
         <v>10</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>24</v>
@@ -699,7 +714,7 @@
         <v>2023</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,10 +734,10 @@
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>29</v>
@@ -731,13 +746,13 @@
         <v>10</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>24</v>
@@ -746,7 +761,7 @@
         <v>2023</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q10" s="0"/>
     </row>
@@ -767,10 +782,10 @@
         <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>31</v>
@@ -779,13 +794,13 @@
         <v>10</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>24</v>
@@ -794,7 +809,7 @@
         <v>2023</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q11" s="0"/>
     </row>
@@ -815,10 +830,10 @@
         <v>5</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>33</v>
@@ -827,13 +842,13 @@
         <v>10</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>24</v>
@@ -842,7 +857,7 @@
         <v>2023</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q12" s="0"/>
     </row>
@@ -863,10 +878,10 @@
         <v>5</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>35</v>
@@ -875,13 +890,13 @@
         <v>10</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>24</v>
@@ -890,7 +905,7 @@
         <v>2023</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q13" s="0"/>
     </row>

</xml_diff>